<commit_message>
Fontawesome icons to sections.
</commit_message>
<xml_diff>
--- a/docs/grants.xlsx
+++ b/docs/grants.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\boloq\Box\CV_Resume\CV\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\boloq\Box\CV_Resume\CV\CVR_BAR\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4F76286-6110-43AE-809E-DCBEB7217F20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3CDBAAF-CF94-4D10-8004-031AD3EC5F85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="grants" sheetId="1" r:id="rId1"/>
@@ -950,18 +950,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
-    </sheetView>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="5" width="45" customWidth="1"/>
-    <col min="6" max="6" width="24" style="1" customWidth="1"/>
-    <col min="7" max="7" width="34.7109375" customWidth="1"/>
+    <col min="6" max="6" width="11.08984375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="24.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -990,7 +988,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1007,7 +1005,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -1033,7 +1031,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1050,7 +1048,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1067,7 +1065,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -1087,7 +1085,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -1107,7 +1105,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
New research info. Moved teaching info around.
</commit_message>
<xml_diff>
--- a/docs/grants.xlsx
+++ b/docs/grants.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
   <si>
     <t xml:space="preserve">what</t>
   </si>
@@ -53,6 +53,9 @@
   </si>
   <si>
     <t xml:space="preserve">February</t>
+  </si>
+  <si>
+    <t xml:space="preserve">,2022</t>
   </si>
   <si>
     <t xml:space="preserve">Department of Ecology and Evolutionary Biology</t>
@@ -373,7 +376,7 @@
   <dimension ref="A1:I1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -423,90 +426,90 @@
         <v>2020</v>
       </c>
       <c r="D2" s="1" t="n">
-        <v>-2021</v>
-      </c>
-      <c r="E2" s="1" t="n">
-        <v>2022</v>
+        <v>2021</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>2021</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E3" s="1" t="n">
         <v>2022</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E4" s="1" t="n">
         <v>2017</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E5" s="1" t="n">
         <v>2017</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E6" s="1" t="n">
         <v>2015</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>